<commit_message>
Update 2022April Sprint Test cases.xlsx
</commit_message>
<xml_diff>
--- a/2022April Sprint Test cases.xlsx
+++ b/2022April Sprint Test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\561625\Documents\GitHub\UiPath-Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1914A64-0B15-4CC8-BD7A-A0662FACBF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DC5EE0-7131-4CCD-B28E-E8951A84C45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="1110" windowWidth="17655" windowHeight="14490" xr2:uid="{A2A8D2E7-EC1F-4C5E-B330-8D00094F85E8}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7440" xr2:uid="{A2A8D2E7-EC1F-4C5E-B330-8D00094F85E8}"/>
   </bookViews>
   <sheets>
     <sheet name="RPA Test Cases" sheetId="1" r:id="rId1"/>
@@ -665,23 +665,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2626AB73-D654-434C-9659-C4D28008D556}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="24.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="49.42578125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="65.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="31.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="3" width="9.1796875" style="3"/>
+    <col min="4" max="4" width="24.54296875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="49.453125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="65.81640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="31.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -704,7 +704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -727,7 +727,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -750,7 +750,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -773,7 +773,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -796,7 +796,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
@@ -819,7 +819,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
@@ -842,7 +842,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -865,7 +865,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
@@ -888,7 +888,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>39</v>
       </c>
@@ -911,7 +911,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>43</v>
       </c>
@@ -934,7 +934,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>46</v>
       </c>
@@ -955,7 +955,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>50</v>
       </c>
@@ -976,7 +976,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Update 2022April Sprint Test
</commit_message>
<xml_diff>
--- a/2022April Sprint Test cases.xlsx
+++ b/2022April Sprint Test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\561625\Documents\GitHub\UiPath-Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333A297A-D4BB-4D88-8AE2-F0E46E9A1A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4536CE7-8616-4CC0-9105-B4734ACBAA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A2A8D2E7-EC1F-4C5E-B330-8D00094F85E8}"/>
+    <workbookView xWindow="6060" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{A2A8D2E7-EC1F-4C5E-B330-8D00094F85E8}"/>
   </bookViews>
   <sheets>
     <sheet name="RPA Test Cases" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
   <si>
     <t>SR#</t>
   </si>
@@ -220,6 +220,27 @@
   </si>
   <si>
     <t>AppliedPatch_CCR</t>
+  </si>
+  <si>
+    <t>Reason: SR Failed to update. Lookup InformationSR0003015453,Beverly Johnson,COR-Bad-Queue-Name,991047..</t>
+  </si>
+  <si>
+    <t>Reason: SR Failed to update. Lookup Information:SR0003015454,COR-Bad-Queue-Name,991048,Beverly Johnson.</t>
+  </si>
+  <si>
+    <t>Reason: SR Failed to update. Lookup InformationSR0003015455,Beverly Johnson,COR-Bad-Queue-Name,991040.,Beverly Johnson.</t>
+  </si>
+  <si>
+    <t>Reason: SR Failed to update. Assigned Queue does not exist in OEC. Lookup information: SR0003015452, COR-Bad-Queue-Name.</t>
+  </si>
+  <si>
+    <t>Reason: SR Failed to update. Assigned Queue does not exist in OEC. Lookup information: SR0003015453, Beverly Johnson, COR-Bad-Queue-Name, 991047. .</t>
+  </si>
+  <si>
+    <t>Reason: SR Failed to update. Assigned Queue does not exist in OEC. Lookup information: SR0003015454, COR-Bad-Queue-Name, 991048, Beverly Johnson.</t>
+  </si>
+  <si>
+    <t>Reason: SR Failed to update. Assigned Queue does not exist in OEC. Lookup information: SR0003015455, Beverly Johnson, COR-Bad-Queue-Name, 991040. , Beverly Johnson.</t>
   </si>
 </sst>
 </file>
@@ -642,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2626AB73-D654-434C-9659-C4D28008D556}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,11 +677,12 @@
     <col min="4" max="4" width="24.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="49.42578125" style="11" customWidth="1"/>
     <col min="6" max="6" width="65.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="31.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="7" width="35.42578125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,11 +701,12 @@
       <c r="F1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -705,8 +728,11 @@
       <c r="G2" s="10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H2" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -725,11 +751,14 @@
       <c r="F3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="13" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H3" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -748,9 +777,14 @@
       <c r="F4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G4" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -769,9 +803,14 @@
       <c r="F5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
@@ -790,9 +829,14 @@
       <c r="F6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G6" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
@@ -811,9 +855,14 @@
       <c r="F7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -835,8 +884,11 @@
       <c r="G8" s="10" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H8" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
@@ -855,11 +907,12 @@
       <c r="F9" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>39</v>
       </c>
@@ -881,8 +934,11 @@
       <c r="G10" s="10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H10" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>43</v>
       </c>
@@ -901,11 +957,12 @@
       <c r="F11" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="10"/>
+      <c r="H11" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>46</v>
       </c>
@@ -925,8 +982,11 @@
       <c r="G12" s="10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>50</v>
       </c>
@@ -943,11 +1003,12 @@
       <c r="F13" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="13"/>
+      <c r="H13" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>57</v>
       </c>
@@ -964,11 +1025,13 @@
       <c r="F14" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="13"/>
+      <c r="H14" s="10" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>